<commit_message>
tour 31 round 1
</commit_message>
<xml_diff>
--- a/my_code/data/scores/courses.xlsx
+++ b/my_code/data/scores/courses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B1E7C2-B220-419C-ADFF-7C433BC4B6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2C72FC-0A1B-441A-ACC7-C4B697E8874A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-90" windowWidth="18450" windowHeight="10980" tabRatio="799" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17968,10 +17968,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9F540D-0219-44DC-A098-2E8716DB0C2D}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -17979,7 +17979,7 @@
     <col min="1" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" s="13" t="s">
         <v>57</v>
       </c>
@@ -17990,7 +17990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -17998,54 +17998,64 @@
         <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -18053,21 +18063,25 @@
         <v>4</v>
       </c>
       <c r="C7" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -18075,10 +18089,12 @@
         <v>4</v>
       </c>
       <c r="C9" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -18086,54 +18102,64 @@
         <v>4</v>
       </c>
       <c r="C10" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.75">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.75">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -18141,67 +18167,77 @@
         <v>4</v>
       </c>
       <c r="C15" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.75">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.75">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.75">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.75">
+        <v>14</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.75">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="10">
         <f>SUM(B2:B19)</f>
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C20" s="10">
         <f>SUM(C2:C19)</f>
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -18212,7 +18248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -18223,7 +18259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -18234,7 +18270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -18245,7 +18281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -18256,7 +18292,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -18267,7 +18303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -18278,7 +18314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -18289,7 +18325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -18300,7 +18336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -18311,7 +18347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -18420,7 +18456,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.75">
@@ -18428,10 +18464,10 @@
         <v>40</v>
       </c>
       <c r="B43" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C43" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.75">
@@ -18439,7 +18475,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
@@ -18450,10 +18486,10 @@
         <v>42</v>
       </c>
       <c r="B45" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="2">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.75">
@@ -18461,10 +18497,10 @@
         <v>43</v>
       </c>
       <c r="B46" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C46" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.75">
@@ -18475,7 +18511,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.75">
@@ -18483,10 +18519,10 @@
         <v>45</v>
       </c>
       <c r="B48" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C48" s="2">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.75">
@@ -18497,7 +18533,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.75">
@@ -18508,7 +18544,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.75">
@@ -18516,10 +18552,10 @@
         <v>48</v>
       </c>
       <c r="B51" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.75">
@@ -18527,10 +18563,10 @@
         <v>49</v>
       </c>
       <c r="B52" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C52" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.75">
@@ -18538,10 +18574,10 @@
         <v>50</v>
       </c>
       <c r="B53" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53" s="2">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.75">
@@ -18552,7 +18588,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="2">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.75">
@@ -18563,7 +18599,7 @@
         <v>4</v>
       </c>
       <c r="C55" s="2">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.75">
@@ -18571,10 +18607,10 @@
         <v>53</v>
       </c>
       <c r="B56" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C56" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.75">
@@ -18582,10 +18618,10 @@
         <v>54</v>
       </c>
       <c r="B57" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C57" s="2">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.75">
@@ -18593,10 +18629,10 @@
         <v>55</v>
       </c>
       <c r="B58" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" s="2">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.75">
@@ -18604,10 +18640,10 @@
         <v>56</v>
       </c>
       <c r="B59" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C59" s="2">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.75">
@@ -18616,7 +18652,7 @@
       </c>
       <c r="B60" s="10">
         <f>SUM(B42:B59)</f>
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C60" s="10">
         <f>SUM(C42:C59)</f>

</xml_diff>

<commit_message>
tour 31 round 2
</commit_message>
<xml_diff>
--- a/my_code/data/scores/courses.xlsx
+++ b/my_code/data/scores/courses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205886DC-EEEE-433D-8007-B00754B11CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EEA3A3-ECF6-469E-9238-197E27511E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-90" windowWidth="18450" windowHeight="10980" tabRatio="799" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17970,8 +17970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9F540D-0219-44DC-A098-2E8716DB0C2D}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:C59"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18241,127 +18241,199 @@
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="2">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="2">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="B25" s="2">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="2">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="2">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="2">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="2">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="2">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="2">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="B34" s="2">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="B35" s="2">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="B36" s="2">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="B37" s="2">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="B38" s="2">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="2">
+        <v>4</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A40" s="9" t="s">
@@ -18369,11 +18441,11 @@
       </c>
       <c r="B40" s="10">
         <f>SUM(B22:B39)</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="C40" s="10">
         <f>SUM(C22:C39)</f>
-        <v>0</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
tour 31 round 3
</commit_message>
<xml_diff>
--- a/my_code/data/scores/courses.xlsx
+++ b/my_code/data/scores/courses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EEA3A3-ECF6-469E-9238-197E27511E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67CF710-8AC2-48F5-81EE-C4CC48AA2AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-90" windowWidth="18450" windowHeight="10980" tabRatio="799" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17970,8 +17970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9F540D-0219-44DC-A098-2E8716DB0C2D}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:C39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18452,127 +18452,199 @@
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="B42" s="2">
+        <v>4</v>
+      </c>
+      <c r="C42" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="B43" s="2">
+        <v>4</v>
+      </c>
+      <c r="C43" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="B44" s="2">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="B45" s="2">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="B46" s="2">
+        <v>5</v>
+      </c>
+      <c r="C46" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="B47" s="2">
+        <v>4</v>
+      </c>
+      <c r="C47" s="2">
+        <v>14</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="B48" s="2">
+        <v>3</v>
+      </c>
+      <c r="C48" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="B49" s="2">
+        <v>4</v>
+      </c>
+      <c r="C49" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="B50" s="2">
+        <v>4</v>
+      </c>
+      <c r="C50" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="2">
+        <v>3</v>
+      </c>
+      <c r="C51" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="2">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="B53" s="2">
+        <v>3</v>
+      </c>
+      <c r="C53" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="2">
+        <v>5</v>
+      </c>
+      <c r="C54" s="2">
+        <v>18</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="B55" s="2">
+        <v>4</v>
+      </c>
+      <c r="C55" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="B56" s="2">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="B57" s="2">
+        <v>3</v>
+      </c>
+      <c r="C57" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="B58" s="2">
+        <v>4</v>
+      </c>
+      <c r="C58" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="B59" s="2">
+        <v>4</v>
+      </c>
+      <c r="C59" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A60" s="9" t="s">
@@ -18580,11 +18652,11 @@
       </c>
       <c r="B60" s="10">
         <f>SUM(B42:B59)</f>
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C60" s="10">
         <f>SUM(C42:C59)</f>
-        <v>0</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>